<commit_message>
update import method user
</commit_message>
<xml_diff>
--- a/public/template/templateuser.xlsx
+++ b/public/template/templateuser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rival\Documents\code\PHU\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E31B22-EC25-4141-AEB6-DC8AF49E231A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9F0FDC-F0ED-4689-A570-ADD2F93AE2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9294E834-221A-436D-A9C3-BB062FBC4D83}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nama</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>travel_company</t>
   </si>
 </sst>
 </file>
@@ -397,15 +400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC33C5C-3A5C-4B20-81DE-36F3945A8335}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,6 +421,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>